<commit_message>
Updating overlay function to enable users to specify icons for each behavioral event.
</commit_message>
<xml_diff>
--- a/Preprocessing/Index Tab Templates.xlsx
+++ b/Preprocessing/Index Tab Templates.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Documents/GitHub/WormTracker3000/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astra/Documents/GitHub/WormTracker3000/Preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92B1D55-71D1-934E-A9E6-F71CF5E6D687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EB40F9-6008-AC42-B997-0D21A1DD6EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="2360" windowWidth="25600" windowHeight="16940" xr2:uid="{44AF9F45-7CA7-644B-9388-3D32C27F2940}"/>
+    <workbookView xWindow="37500" yWindow="640" windowWidth="36000" windowHeight="20940" activeTab="3" xr2:uid="{44AF9F45-7CA7-644B-9388-3D32C27F2940}"/>
   </bookViews>
   <sheets>
     <sheet name="Chemotaxis Index" sheetId="1" r:id="rId1"/>
     <sheet name="Thermotaxis Index " sheetId="2" r:id="rId2"/>
     <sheet name="Custom Linear Assay Index " sheetId="3" r:id="rId3"/>
+    <sheet name="Overlay" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>Number of Worms</t>
   </si>
@@ -83,6 +84,15 @@
   </si>
   <si>
     <t>T(s) XCoord</t>
+  </si>
+  <si>
+    <t>Frame</t>
+  </si>
+  <si>
+    <t>Behavior</t>
+  </si>
+  <si>
+    <t>Icon</t>
   </si>
 </sst>
 </file>
@@ -141,9 +151,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -181,7 +191,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -287,7 +297,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -429,7 +439,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -439,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0CF6085-3659-9841-BB82-F165B4735852}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -670,4 +680,33 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041A9669-D2E2-0449-BA54-AF11F84CE85E}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>